<commit_message>
nmv 23 01 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.6.xlsx
@@ -1,40 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
-  <workbookPr showObjects="none"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B2B5F8-6DBF-477C-9310-27BA191BF4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F128FD63-1A6D-4070-9FCC-E557E32C1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4.1" sheetId="15" r:id="rId1"/>
-    <sheet name="total 4.1 to 4.6" sheetId="7" r:id="rId2"/>
+    <sheet name="4.2" sheetId="16" r:id="rId2"/>
+    <sheet name="total 4.1 to 4.6" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="148">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1539,6 +1532,150 @@
   </si>
   <si>
     <t>4.1.11.4 :</t>
+  </si>
+  <si>
+    <t>4.2.1.1 :</t>
+  </si>
+  <si>
+    <t>4.2.1.2 :</t>
+  </si>
+  <si>
+    <t>4.2.1.3 :</t>
+  </si>
+  <si>
+    <t>4.2.1.4 :</t>
+  </si>
+  <si>
+    <t>4.2.1.5 :</t>
+  </si>
+  <si>
+    <t>4.2.2.1 :</t>
+  </si>
+  <si>
+    <t>4.2.2.2 :</t>
+  </si>
+  <si>
+    <t>4.2.2.3 :</t>
+  </si>
+  <si>
+    <t>4.2.2.4 :</t>
+  </si>
+  <si>
+    <t>4.2.3.1 :</t>
+  </si>
+  <si>
+    <t>4.2.3.2 :</t>
+  </si>
+  <si>
+    <t>4.2.3.3 :</t>
+  </si>
+  <si>
+    <t>4.2.3.4 :</t>
+  </si>
+  <si>
+    <t>4.2.4.1 :</t>
+  </si>
+  <si>
+    <t>4.2.4.2 :</t>
+  </si>
+  <si>
+    <t>4.2.4.3 :</t>
+  </si>
+  <si>
+    <t>4.2.4.4 :</t>
+  </si>
+  <si>
+    <t>4.2.5.1 :</t>
+  </si>
+  <si>
+    <t>4.2.5.2 :</t>
+  </si>
+  <si>
+    <t>4.2.5.3 :</t>
+  </si>
+  <si>
+    <t>4.2.5.4 :</t>
+  </si>
+  <si>
+    <t>4.2.5.5 :</t>
+  </si>
+  <si>
+    <t>4.2.5.6 :</t>
+  </si>
+  <si>
+    <t>4.2.6.1 :</t>
+  </si>
+  <si>
+    <t>4.2.6.2 :</t>
+  </si>
+  <si>
+    <t>4.2.6.3 :</t>
+  </si>
+  <si>
+    <t>4.2.6.4 :</t>
+  </si>
+  <si>
+    <t>4.2.6.5 :</t>
+  </si>
+  <si>
+    <t>4.2.7.1 :</t>
+  </si>
+  <si>
+    <t>4.2.7.2 :</t>
+  </si>
+  <si>
+    <t>4.2.7.3 :</t>
+  </si>
+  <si>
+    <t>4.2.7.4 :</t>
+  </si>
+  <si>
+    <t>4.2.8.1 :</t>
+  </si>
+  <si>
+    <t>4.2.8.2 :</t>
+  </si>
+  <si>
+    <t>4.2.8.3 :</t>
+  </si>
+  <si>
+    <t>4.2.9.1 :</t>
+  </si>
+  <si>
+    <t>4.2.9.2 :</t>
+  </si>
+  <si>
+    <t>4.2.9.3 :</t>
+  </si>
+  <si>
+    <t>4.2.9.4 :</t>
+  </si>
+  <si>
+    <t>4.2.9.5 :</t>
+  </si>
+  <si>
+    <t>4.2.9.6 :</t>
+  </si>
+  <si>
+    <t>4.2.10.1 :</t>
+  </si>
+  <si>
+    <t>4.2.10.2 :</t>
+  </si>
+  <si>
+    <t>4.2.10.3 :</t>
+  </si>
+  <si>
+    <t>4.2.10.4 :</t>
+  </si>
+  <si>
+    <t>4.2.11.1 :</t>
+  </si>
+  <si>
+    <t>4.2.11.2 :</t>
+  </si>
+  <si>
+    <t>4.2.11.3 :</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -1850,13 +1987,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2139,9 +2273,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M52" sqref="M52"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49:K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2367,7 @@
       <c r="L2" s="3">
         <v>53</v>
       </c>
-      <c r="M2" s="35"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2272,7 +2406,7 @@
       <c r="L3" s="3">
         <v>53</v>
       </c>
-      <c r="M3" s="35"/>
+      <c r="M3" s="34"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -2311,7 +2445,7 @@
       <c r="L4" s="3">
         <v>58</v>
       </c>
-      <c r="M4" s="35"/>
+      <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2350,7 +2484,7 @@
       <c r="L5" s="3">
         <v>57</v>
       </c>
-      <c r="M5" s="35"/>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -2389,7 +2523,7 @@
       <c r="L6" s="3">
         <v>55</v>
       </c>
-      <c r="M6" s="35"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2428,9 +2562,9 @@
       <c r="L7" s="3">
         <v>56</v>
       </c>
-      <c r="M7" s="35"/>
-    </row>
-    <row r="8" spans="1:13" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -2467,9 +2601,9 @@
       <c r="L8" s="3">
         <v>57</v>
       </c>
-      <c r="M8" s="35"/>
-    </row>
-    <row r="9" spans="1:13" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>61</v>
       </c>
@@ -2506,9 +2640,9 @@
       <c r="L9" s="3">
         <v>58</v>
       </c>
-      <c r="M9" s="35"/>
-    </row>
-    <row r="10" spans="1:13" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>62</v>
       </c>
@@ -2545,9 +2679,9 @@
       <c r="L10" s="3">
         <v>81</v>
       </c>
-      <c r="M10" s="35"/>
-    </row>
-    <row r="11" spans="1:13" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>63</v>
       </c>
@@ -2584,9 +2718,9 @@
       <c r="L11" s="3">
         <v>57</v>
       </c>
-      <c r="M11" s="35"/>
-    </row>
-    <row r="12" spans="1:13" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M11" s="34"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>64</v>
       </c>
@@ -2623,9 +2757,9 @@
       <c r="L12" s="3">
         <v>56</v>
       </c>
-      <c r="M12" s="35"/>
-    </row>
-    <row r="13" spans="1:13" s="34" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M12" s="34"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>65</v>
       </c>
@@ -2662,7 +2796,7 @@
       <c r="L13" s="3">
         <v>58</v>
       </c>
-      <c r="M13" s="35"/>
+      <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -2701,7 +2835,7 @@
       <c r="L14" s="3">
         <v>29</v>
       </c>
-      <c r="M14" s="36"/>
+      <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -2740,7 +2874,7 @@
       <c r="L15" s="3">
         <v>56</v>
       </c>
-      <c r="M15" s="36"/>
+      <c r="M15" s="34"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -2779,7 +2913,7 @@
       <c r="L16" s="3">
         <v>56</v>
       </c>
-      <c r="M16" s="36"/>
+      <c r="M16" s="34"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -2818,7 +2952,7 @@
       <c r="L17" s="3">
         <v>53</v>
       </c>
-      <c r="M17" s="36"/>
+      <c r="M17" s="34"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -2857,7 +2991,7 @@
       <c r="L18" s="3">
         <v>42</v>
       </c>
-      <c r="M18" s="36"/>
+      <c r="M18" s="34"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -2896,7 +3030,7 @@
       <c r="L19" s="3">
         <v>54</v>
       </c>
-      <c r="M19" s="36"/>
+      <c r="M19" s="34"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -2935,7 +3069,7 @@
       <c r="L20" s="3">
         <v>57</v>
       </c>
-      <c r="M20" s="36"/>
+      <c r="M20" s="34"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -2974,7 +3108,7 @@
       <c r="L21" s="3">
         <v>55</v>
       </c>
-      <c r="M21" s="36"/>
+      <c r="M21" s="34"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -3013,7 +3147,7 @@
       <c r="L22" s="3">
         <v>59</v>
       </c>
-      <c r="M22" s="36"/>
+      <c r="M22" s="34"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -3052,7 +3186,7 @@
       <c r="L23" s="3">
         <v>53</v>
       </c>
-      <c r="M23" s="36"/>
+      <c r="M23" s="34"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -3091,7 +3225,7 @@
       <c r="L24" s="3">
         <v>58</v>
       </c>
-      <c r="M24" s="36"/>
+      <c r="M24" s="34"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -3130,7 +3264,7 @@
       <c r="L25" s="3">
         <v>73</v>
       </c>
-      <c r="M25" s="36"/>
+      <c r="M25" s="34"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -3169,7 +3303,7 @@
       <c r="L26" s="3">
         <v>53</v>
       </c>
-      <c r="M26" s="36"/>
+      <c r="M26" s="34"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -3208,7 +3342,7 @@
       <c r="L27" s="3">
         <v>61</v>
       </c>
-      <c r="M27" s="36"/>
+      <c r="M27" s="34"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -3247,7 +3381,7 @@
       <c r="L28" s="3">
         <v>60</v>
       </c>
-      <c r="M28" s="36"/>
+      <c r="M28" s="34"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -3286,7 +3420,7 @@
       <c r="L29" s="3">
         <v>37</v>
       </c>
-      <c r="M29" s="36"/>
+      <c r="M29" s="34"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -3325,7 +3459,7 @@
       <c r="L30" s="3">
         <v>56</v>
       </c>
-      <c r="M30" s="36"/>
+      <c r="M30" s="34"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -3364,7 +3498,7 @@
       <c r="L31" s="3">
         <v>55</v>
       </c>
-      <c r="M31" s="36"/>
+      <c r="M31" s="34"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -3403,7 +3537,7 @@
       <c r="L32" s="3">
         <v>52</v>
       </c>
-      <c r="M32" s="36"/>
+      <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -3442,7 +3576,7 @@
       <c r="L33" s="3">
         <v>61</v>
       </c>
-      <c r="M33" s="36"/>
+      <c r="M33" s="34"/>
     </row>
     <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -3481,7 +3615,7 @@
       <c r="L34" s="3">
         <v>59</v>
       </c>
-      <c r="M34" s="36"/>
+      <c r="M34" s="34"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
@@ -3520,7 +3654,7 @@
       <c r="L35" s="3">
         <v>35</v>
       </c>
-      <c r="M35" s="36"/>
+      <c r="M35" s="34"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
@@ -3559,7 +3693,7 @@
       <c r="L36" s="3">
         <v>58</v>
       </c>
-      <c r="M36" s="36"/>
+      <c r="M36" s="34"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -3598,7 +3732,7 @@
       <c r="L37" s="3">
         <v>54</v>
       </c>
-      <c r="M37" s="36"/>
+      <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
@@ -3637,7 +3771,7 @@
       <c r="L38" s="3">
         <v>77</v>
       </c>
-      <c r="M38" s="36"/>
+      <c r="M38" s="34"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -3676,7 +3810,7 @@
       <c r="L39" s="3">
         <v>54</v>
       </c>
-      <c r="M39" s="36"/>
+      <c r="M39" s="34"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
@@ -3715,7 +3849,7 @@
       <c r="L40" s="3">
         <v>57</v>
       </c>
-      <c r="M40" s="36"/>
+      <c r="M40" s="34"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -3754,7 +3888,7 @@
       <c r="L41" s="3">
         <v>56</v>
       </c>
-      <c r="M41" s="36"/>
+      <c r="M41" s="34"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -3793,7 +3927,7 @@
       <c r="L42" s="3">
         <v>57</v>
       </c>
-      <c r="M42" s="36"/>
+      <c r="M42" s="34"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -3832,7 +3966,7 @@
       <c r="L43" s="3">
         <v>43</v>
       </c>
-      <c r="M43" s="36"/>
+      <c r="M43" s="34"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -3871,7 +4005,7 @@
       <c r="L44" s="3">
         <v>53</v>
       </c>
-      <c r="M44" s="36"/>
+      <c r="M44" s="34"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
@@ -3910,7 +4044,7 @@
       <c r="L45" s="3">
         <v>54</v>
       </c>
-      <c r="M45" s="36"/>
+      <c r="M45" s="34"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
@@ -3949,7 +4083,7 @@
       <c r="L46" s="3">
         <v>57</v>
       </c>
-      <c r="M46" s="36"/>
+      <c r="M46" s="34"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
@@ -3988,7 +4122,7 @@
       <c r="L47" s="3">
         <v>64</v>
       </c>
-      <c r="M47" s="36"/>
+      <c r="M47" s="34"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
@@ -4038,12 +4172,12 @@
         <f t="shared" si="0"/>
         <v>2557</v>
       </c>
-      <c r="M48" s="36"/>
+      <c r="M48" s="34"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
       <c r="E49" t="s">
         <v>12</v>
       </c>
@@ -4055,8 +4189,8 @@
         <f>B48-C48</f>
         <v>238</v>
       </c>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
@@ -4148,6 +4282,2045 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16770CAE-DF7A-416E-83DB-16CCD44DE18D}">
+  <dimension ref="A1:L60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>45</v>
+      </c>
+      <c r="K2" s="3">
+        <v>50</v>
+      </c>
+      <c r="L2" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="3">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>40</v>
+      </c>
+      <c r="K3" s="3">
+        <v>50</v>
+      </c>
+      <c r="L3" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>41</v>
+      </c>
+      <c r="K4" s="3">
+        <v>50</v>
+      </c>
+      <c r="L4" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>42</v>
+      </c>
+      <c r="K5" s="3">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="3">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>43</v>
+      </c>
+      <c r="K6" s="3">
+        <v>66</v>
+      </c>
+      <c r="L6" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>4</v>
+      </c>
+      <c r="J7" s="3">
+        <v>39</v>
+      </c>
+      <c r="K7" s="3">
+        <v>50</v>
+      </c>
+      <c r="L7" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>43</v>
+      </c>
+      <c r="K8" s="3">
+        <v>50</v>
+      </c>
+      <c r="L8" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>36</v>
+      </c>
+      <c r="K9" s="3">
+        <v>50</v>
+      </c>
+      <c r="L9" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>6</v>
+      </c>
+      <c r="G10" s="3">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>44</v>
+      </c>
+      <c r="K10" s="3">
+        <v>54</v>
+      </c>
+      <c r="L10" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="3">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7</v>
+      </c>
+      <c r="G11" s="3">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>34</v>
+      </c>
+      <c r="K11" s="3">
+        <v>50</v>
+      </c>
+      <c r="L11" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>4</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>42</v>
+      </c>
+      <c r="K12" s="3">
+        <v>50</v>
+      </c>
+      <c r="L12" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="3">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>37</v>
+      </c>
+      <c r="K13" s="3">
+        <v>50</v>
+      </c>
+      <c r="L13" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="3">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>51</v>
+      </c>
+      <c r="K14" s="3">
+        <v>66</v>
+      </c>
+      <c r="L14" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="3">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4</v>
+      </c>
+      <c r="G15" s="3">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>42</v>
+      </c>
+      <c r="K15" s="3">
+        <v>50</v>
+      </c>
+      <c r="L15" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="3">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3">
+        <v>41</v>
+      </c>
+      <c r="K16" s="3">
+        <v>50</v>
+      </c>
+      <c r="L16" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="3">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>7</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>35</v>
+      </c>
+      <c r="K17" s="3">
+        <v>50</v>
+      </c>
+      <c r="L17" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>5</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>39</v>
+      </c>
+      <c r="K18" s="3">
+        <v>48</v>
+      </c>
+      <c r="L18" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="3">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>6</v>
+      </c>
+      <c r="G19" s="3">
+        <v>8</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>36</v>
+      </c>
+      <c r="K19" s="3">
+        <v>50</v>
+      </c>
+      <c r="L19" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="3">
+        <v>8</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>6</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>36</v>
+      </c>
+      <c r="K20" s="3">
+        <v>50</v>
+      </c>
+      <c r="L20" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="3">
+        <v>8</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>5</v>
+      </c>
+      <c r="G21" s="3">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3">
+        <v>40</v>
+      </c>
+      <c r="K21" s="3">
+        <v>50</v>
+      </c>
+      <c r="L21" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="3">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>5</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>40</v>
+      </c>
+      <c r="K22" s="3">
+        <v>50</v>
+      </c>
+      <c r="L22" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="3">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>8</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>37</v>
+      </c>
+      <c r="K23" s="3">
+        <v>50</v>
+      </c>
+      <c r="L23" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="3">
+        <v>14</v>
+      </c>
+      <c r="C24" s="3">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>11</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>52</v>
+      </c>
+      <c r="K24" s="3">
+        <v>72</v>
+      </c>
+      <c r="L24" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="3">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>7</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3">
+        <v>37</v>
+      </c>
+      <c r="K25" s="3">
+        <v>50</v>
+      </c>
+      <c r="L25" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3">
+        <v>35</v>
+      </c>
+      <c r="K26" s="3">
+        <v>50</v>
+      </c>
+      <c r="L26" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>7</v>
+      </c>
+      <c r="G27" s="3">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3">
+        <v>40</v>
+      </c>
+      <c r="K27" s="3">
+        <v>50</v>
+      </c>
+      <c r="L27" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="3">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>8</v>
+      </c>
+      <c r="G28" s="3">
+        <v>3</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>36</v>
+      </c>
+      <c r="K28" s="3">
+        <v>50</v>
+      </c>
+      <c r="L28" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="3">
+        <v>10</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3">
+        <v>5</v>
+      </c>
+      <c r="H29" s="3">
+        <v>2</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>50</v>
+      </c>
+      <c r="K29" s="3">
+        <v>68</v>
+      </c>
+      <c r="L29" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>6</v>
+      </c>
+      <c r="G30" s="3">
+        <v>2</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>42</v>
+      </c>
+      <c r="K30" s="3">
+        <v>50</v>
+      </c>
+      <c r="L30" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="3">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>6</v>
+      </c>
+      <c r="G31" s="3">
+        <v>3</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>39</v>
+      </c>
+      <c r="K31" s="3">
+        <v>50</v>
+      </c>
+      <c r="L31" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="3">
+        <v>15</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
+        <v>7</v>
+      </c>
+      <c r="G32" s="3">
+        <v>3</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>27</v>
+      </c>
+      <c r="K32" s="3">
+        <v>50</v>
+      </c>
+      <c r="L32" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="3">
+        <v>6</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>6</v>
+      </c>
+      <c r="G33" s="3">
+        <v>5</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>29</v>
+      </c>
+      <c r="K33" s="3">
+        <v>39</v>
+      </c>
+      <c r="L33" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="3">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <v>41</v>
+      </c>
+      <c r="K34" s="3">
+        <v>50</v>
+      </c>
+      <c r="L34" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" s="3">
+        <v>4</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>5</v>
+      </c>
+      <c r="G35" s="3">
+        <v>4</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <v>41</v>
+      </c>
+      <c r="K35" s="3">
+        <v>50</v>
+      </c>
+      <c r="L35" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>8</v>
+      </c>
+      <c r="G36" s="3">
+        <v>5</v>
+      </c>
+      <c r="H36" s="3">
+        <v>2</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
+      <c r="J36" s="3">
+        <v>50</v>
+      </c>
+      <c r="K36" s="3">
+        <v>61</v>
+      </c>
+      <c r="L36" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="3">
+        <v>10</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>39</v>
+      </c>
+      <c r="K37" s="3">
+        <v>50</v>
+      </c>
+      <c r="L37" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="3">
+        <v>7</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>6</v>
+      </c>
+      <c r="G38" s="3">
+        <v>3</v>
+      </c>
+      <c r="H38" s="3">
+        <v>1</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>38</v>
+      </c>
+      <c r="K38" s="3">
+        <v>50</v>
+      </c>
+      <c r="L38" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="3">
+        <v>5</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>9</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
+      <c r="J39" s="3">
+        <v>37</v>
+      </c>
+      <c r="K39" s="3">
+        <v>50</v>
+      </c>
+      <c r="L39" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="3">
+        <v>5</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>8</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="3">
+        <v>38</v>
+      </c>
+      <c r="K40" s="3">
+        <v>50</v>
+      </c>
+      <c r="L40" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="3">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>6</v>
+      </c>
+      <c r="G41" s="3">
+        <v>5</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2</v>
+      </c>
+      <c r="J41" s="3">
+        <v>40</v>
+      </c>
+      <c r="K41" s="3">
+        <v>50</v>
+      </c>
+      <c r="L41" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="3">
+        <v>3</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3">
+        <v>9</v>
+      </c>
+      <c r="G42" s="3">
+        <v>2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0</v>
+      </c>
+      <c r="J42" s="3">
+        <v>42</v>
+      </c>
+      <c r="K42" s="3">
+        <v>54</v>
+      </c>
+      <c r="L42" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" s="3">
+        <v>7</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+      <c r="F43" s="3">
+        <v>5</v>
+      </c>
+      <c r="G43" s="3">
+        <v>5</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" s="3">
+        <v>39</v>
+      </c>
+      <c r="K43" s="3">
+        <v>50</v>
+      </c>
+      <c r="L43" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" s="3">
+        <v>9</v>
+      </c>
+      <c r="C44" s="3">
+        <v>3</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>6</v>
+      </c>
+      <c r="G44" s="3">
+        <v>2</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>38</v>
+      </c>
+      <c r="K44" s="3">
+        <v>50</v>
+      </c>
+      <c r="L44" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" s="3">
+        <v>6</v>
+      </c>
+      <c r="C45" s="3">
+        <v>4</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3">
+        <v>6</v>
+      </c>
+      <c r="G45" s="3">
+        <v>3</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0</v>
+      </c>
+      <c r="J45" s="3">
+        <v>42</v>
+      </c>
+      <c r="K45" s="3">
+        <v>50</v>
+      </c>
+      <c r="L45" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="3">
+        <v>3</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>6</v>
+      </c>
+      <c r="G46" s="3">
+        <v>7</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3">
+        <v>50</v>
+      </c>
+      <c r="K46" s="3">
+        <v>59</v>
+      </c>
+      <c r="L46" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="3">
+        <v>6</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3">
+        <v>5</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <v>6</v>
+      </c>
+      <c r="G47" s="3">
+        <v>8</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0</v>
+      </c>
+      <c r="J47" s="3">
+        <v>34</v>
+      </c>
+      <c r="K47" s="3">
+        <v>50</v>
+      </c>
+      <c r="L47" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="3">
+        <v>10</v>
+      </c>
+      <c r="C48" s="3">
+        <v>3</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>9</v>
+      </c>
+      <c r="G48" s="3">
+        <v>4</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>2</v>
+      </c>
+      <c r="J48" s="3">
+        <v>34</v>
+      </c>
+      <c r="K48" s="3">
+        <v>50</v>
+      </c>
+      <c r="L48" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="3">
+        <v>8</v>
+      </c>
+      <c r="C49" s="3">
+        <v>3</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>8</v>
+      </c>
+      <c r="G49" s="3">
+        <v>2</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
+      <c r="J49" s="3">
+        <v>48</v>
+      </c>
+      <c r="K49" s="3">
+        <v>61</v>
+      </c>
+      <c r="L49" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="35">
+        <v>48</v>
+      </c>
+      <c r="B50" s="35">
+        <f>SUM(B2:B49)</f>
+        <v>317</v>
+      </c>
+      <c r="C50" s="35">
+        <f t="shared" ref="C50:L50" si="0">SUM(C2:C49)</f>
+        <v>65</v>
+      </c>
+      <c r="D50" s="35">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E50" s="35">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F50" s="35">
+        <f t="shared" si="0"/>
+        <v>307</v>
+      </c>
+      <c r="G50" s="35">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="H50" s="35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I50" s="35">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J50" s="35">
+        <f t="shared" si="0"/>
+        <v>1921</v>
+      </c>
+      <c r="K50" s="35">
+        <f t="shared" si="0"/>
+        <v>2498</v>
+      </c>
+      <c r="L50" s="35">
+        <f t="shared" si="0"/>
+        <v>2768</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D51" s="34"/>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51">
+        <f>G50</f>
+        <v>178</v>
+      </c>
+      <c r="J51">
+        <f>B50-C50</f>
+        <v>252</v>
+      </c>
+      <c r="K51" s="34"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52">
+        <f>B50</f>
+        <v>317</v>
+      </c>
+      <c r="J52">
+        <f>D50-E50</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53">
+        <v>14</v>
+      </c>
+      <c r="J53">
+        <f>F59</f>
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54">
+        <v>7</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55">
+        <f>SUM(J51:J54)</f>
+        <v>2768</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f>SUM(F51:F55)</f>
+        <v>516</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57">
+        <f>K50-F56</f>
+        <v>1982</v>
+      </c>
+      <c r="J57">
+        <f>J55-L50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F58" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f>F57+F56</f>
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f>F59-K50</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K31"/>
   <sheetViews>
@@ -4340,7 +6513,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
       <c r="K8" s="17">
-        <f t="shared" ref="F8:K8" si="0">SUM(K3:K7)</f>
+        <f t="shared" ref="K8" si="0">SUM(K3:K7)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nmv 08 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.6.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F128FD63-1A6D-4070-9FCC-E557E32C1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02802691-95F9-404E-A651-AD7F9B965653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4.1" sheetId="15" r:id="rId1"/>
     <sheet name="4.2" sheetId="16" r:id="rId2"/>
-    <sheet name="total 4.1 to 4.6" sheetId="7" r:id="rId3"/>
+    <sheet name="4.3" sheetId="17" r:id="rId3"/>
+    <sheet name="total 4.1 to 4.6" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="185">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1676,6 +1677,117 @@
   </si>
   <si>
     <t>4.2.11.3 :</t>
+  </si>
+  <si>
+    <t>4.3.1.1 :</t>
+  </si>
+  <si>
+    <t>4.3.2.1 :</t>
+  </si>
+  <si>
+    <t>4.3.2.2 :</t>
+  </si>
+  <si>
+    <t>4.3.2.3 :</t>
+  </si>
+  <si>
+    <t>4.3.3.1 :</t>
+  </si>
+  <si>
+    <t>4.3.3.2 :</t>
+  </si>
+  <si>
+    <t>4.3.4.1 :</t>
+  </si>
+  <si>
+    <t>4.3.4.2 :</t>
+  </si>
+  <si>
+    <t>4.3.4.3 :</t>
+  </si>
+  <si>
+    <t>4.3.5.1 :</t>
+  </si>
+  <si>
+    <t>4.3.6.1 :</t>
+  </si>
+  <si>
+    <t>4.3.6.2 :</t>
+  </si>
+  <si>
+    <t>4.3.7.1 :</t>
+  </si>
+  <si>
+    <t>4.3.7.2 :</t>
+  </si>
+  <si>
+    <t>4.3.8.1 :</t>
+  </si>
+  <si>
+    <t>4.3.9.1 :</t>
+  </si>
+  <si>
+    <t>4.3.9.2 :</t>
+  </si>
+  <si>
+    <t>4.3.10.1 :</t>
+  </si>
+  <si>
+    <t>4.3.10.2 :</t>
+  </si>
+  <si>
+    <t>4.3.10.3 :</t>
+  </si>
+  <si>
+    <t>4.3.11.1 :</t>
+  </si>
+  <si>
+    <t>4.3.11.2 :</t>
+  </si>
+  <si>
+    <t>4.3.11.3 :</t>
+  </si>
+  <si>
+    <t>4.3.11.4 :</t>
+  </si>
+  <si>
+    <t>4.3.11.5 :</t>
+  </si>
+  <si>
+    <t>4.3.12.1 :</t>
+  </si>
+  <si>
+    <t>4.3.12.2 :</t>
+  </si>
+  <si>
+    <t>4.3.12.3 :</t>
+  </si>
+  <si>
+    <t>4.3.13.1 :</t>
+  </si>
+  <si>
+    <t>4.3.13.2 :</t>
+  </si>
+  <si>
+    <t>4.3.13.3 :</t>
+  </si>
+  <si>
+    <t>4.3.13.4 :</t>
+  </si>
+  <si>
+    <t>4.3.13.5 :</t>
+  </si>
+  <si>
+    <t>4.3.13.6 :</t>
+  </si>
+  <si>
+    <t>4.3.13.7 :</t>
+  </si>
+  <si>
+    <t>4.3.13.8 :</t>
+  </si>
+  <si>
+    <t>36</t>
   </si>
 </sst>
 </file>
@@ -4285,9 +4397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16770CAE-DF7A-416E-83DB-16CCD44DE18D}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51:J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6321,6 +6433,1576 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DC1F4F-BBB6-40F8-A352-CB08F5EFE478}">
+  <dimension ref="A1:L48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>62</v>
+      </c>
+      <c r="K2" s="3">
+        <v>65</v>
+      </c>
+      <c r="L2" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="3">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>33</v>
+      </c>
+      <c r="K3" s="3">
+        <v>50</v>
+      </c>
+      <c r="L3" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="3">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>36</v>
+      </c>
+      <c r="K4" s="3">
+        <v>50</v>
+      </c>
+      <c r="L4" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>20</v>
+      </c>
+      <c r="K5" s="3">
+        <v>30</v>
+      </c>
+      <c r="L5" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>41</v>
+      </c>
+      <c r="K6" s="3">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="3">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>58</v>
+      </c>
+      <c r="K7" s="3">
+        <v>78</v>
+      </c>
+      <c r="L7" s="3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="3">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>35</v>
+      </c>
+      <c r="K8" s="3">
+        <v>50</v>
+      </c>
+      <c r="L8" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="3">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>34</v>
+      </c>
+      <c r="K9" s="3">
+        <v>50</v>
+      </c>
+      <c r="L9" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="3">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>44</v>
+      </c>
+      <c r="K10" s="3">
+        <v>67</v>
+      </c>
+      <c r="L10" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="3">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>59</v>
+      </c>
+      <c r="K11" s="3">
+        <v>76</v>
+      </c>
+      <c r="L11" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>39</v>
+      </c>
+      <c r="K12" s="3">
+        <v>50</v>
+      </c>
+      <c r="L12" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>46</v>
+      </c>
+      <c r="K13" s="3">
+        <v>56</v>
+      </c>
+      <c r="L13" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>45</v>
+      </c>
+      <c r="K14" s="3">
+        <v>50</v>
+      </c>
+      <c r="L14" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>55</v>
+      </c>
+      <c r="K15" s="3">
+        <v>56</v>
+      </c>
+      <c r="L15" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="3">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>14</v>
+      </c>
+      <c r="K16" s="3">
+        <v>37</v>
+      </c>
+      <c r="L16" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="3">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>39</v>
+      </c>
+      <c r="K17" s="3">
+        <v>50</v>
+      </c>
+      <c r="L17" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" s="3">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>32</v>
+      </c>
+      <c r="K18" s="3">
+        <v>46</v>
+      </c>
+      <c r="L18" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>33</v>
+      </c>
+      <c r="K19" s="3">
+        <v>50</v>
+      </c>
+      <c r="L19" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="3">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>33</v>
+      </c>
+      <c r="K20" s="3">
+        <v>50</v>
+      </c>
+      <c r="L20" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="3">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>25</v>
+      </c>
+      <c r="K21" s="3">
+        <v>35</v>
+      </c>
+      <c r="L21" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="3">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>6</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>36</v>
+      </c>
+      <c r="K22" s="3">
+        <v>50</v>
+      </c>
+      <c r="L22" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="3">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>6</v>
+      </c>
+      <c r="G23" s="3">
+        <v>3</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>39</v>
+      </c>
+      <c r="K23" s="3">
+        <v>50</v>
+      </c>
+      <c r="L23" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="3">
+        <v>8</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>6</v>
+      </c>
+      <c r="G24" s="3">
+        <v>5</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>38</v>
+      </c>
+      <c r="K24" s="3">
+        <v>50</v>
+      </c>
+      <c r="L24" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="3">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>5</v>
+      </c>
+      <c r="G25" s="3">
+        <v>7</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>36</v>
+      </c>
+      <c r="K25" s="3">
+        <v>50</v>
+      </c>
+      <c r="L25" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3">
+        <v>5</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <v>53</v>
+      </c>
+      <c r="K26" s="3">
+        <v>69</v>
+      </c>
+      <c r="L26" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" s="3">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <v>39</v>
+      </c>
+      <c r="K27" s="3">
+        <v>50</v>
+      </c>
+      <c r="L27" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="3">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>39</v>
+      </c>
+      <c r="K28" s="3">
+        <v>50</v>
+      </c>
+      <c r="L28" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="3">
+        <v>7</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>25</v>
+      </c>
+      <c r="K29" s="3">
+        <v>33</v>
+      </c>
+      <c r="L29" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" s="3">
+        <v>7</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>7</v>
+      </c>
+      <c r="G30" s="3">
+        <v>2</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>39</v>
+      </c>
+      <c r="K30" s="3">
+        <v>50</v>
+      </c>
+      <c r="L30" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="3">
+        <v>8</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>36</v>
+      </c>
+      <c r="K31" s="3">
+        <v>50</v>
+      </c>
+      <c r="L31" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" s="3">
+        <v>8</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>8</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>36</v>
+      </c>
+      <c r="K32" s="3">
+        <v>50</v>
+      </c>
+      <c r="L32" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="3">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>6</v>
+      </c>
+      <c r="G33" s="3">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>38</v>
+      </c>
+      <c r="K33" s="3">
+        <v>50</v>
+      </c>
+      <c r="L33" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="3">
+        <v>11</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>9</v>
+      </c>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <v>33</v>
+      </c>
+      <c r="K34" s="3">
+        <v>50</v>
+      </c>
+      <c r="L34" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="3">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3">
+        <v>5</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <v>36</v>
+      </c>
+      <c r="K35" s="3">
+        <v>50</v>
+      </c>
+      <c r="L35" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" s="3">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>5</v>
+      </c>
+      <c r="G36" s="3">
+        <v>3</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
+      <c r="J36" s="3">
+        <v>39</v>
+      </c>
+      <c r="K36" s="3">
+        <v>50</v>
+      </c>
+      <c r="L36" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B37" s="3">
+        <v>8</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>7</v>
+      </c>
+      <c r="G37" s="3">
+        <v>3</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3">
+        <v>32</v>
+      </c>
+      <c r="K37" s="3">
+        <v>46</v>
+      </c>
+      <c r="L37" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="35">
+        <v>356</v>
+      </c>
+      <c r="C38" s="35">
+        <v>29</v>
+      </c>
+      <c r="D38" s="35">
+        <v>25</v>
+      </c>
+      <c r="E38" s="35">
+        <v>1</v>
+      </c>
+      <c r="F38" s="35">
+        <v>16</v>
+      </c>
+      <c r="G38" s="35">
+        <v>67</v>
+      </c>
+      <c r="H38" s="35">
+        <v>0</v>
+      </c>
+      <c r="I38" s="35">
+        <v>2</v>
+      </c>
+      <c r="J38" s="35">
+        <v>1377</v>
+      </c>
+      <c r="K38" s="35">
+        <v>1844</v>
+      </c>
+      <c r="L38" s="35">
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <f>G38</f>
+        <v>67</v>
+      </c>
+      <c r="J39">
+        <f>B38-C38</f>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <f>B38</f>
+        <v>356</v>
+      </c>
+      <c r="J40">
+        <f>D38-E38</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <v>15</v>
+      </c>
+      <c r="J41">
+        <f>F47</f>
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43">
+        <f>SUM(J39:J42)</f>
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f>SUM(F39:F43)</f>
+        <v>448</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>46</v>
+      </c>
+      <c r="F45">
+        <f>K38-F44</f>
+        <v>1396</v>
+      </c>
+      <c r="J45">
+        <f>J43-L38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F46" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f>F45+F44</f>
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f>F47-K38</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K31"/>
   <sheetViews>
@@ -6818,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="99" x14ac:dyDescent="0.4">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
@@ -6839,7 +8521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="99" x14ac:dyDescent="0.4">
       <c r="B28" s="12" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
nmv 24 02 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.6.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02802691-95F9-404E-A651-AD7F9B965653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572D4125-F00A-4C05-BCE9-C32DEF16A737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4.1" sheetId="15" r:id="rId1"/>
     <sheet name="4.2" sheetId="16" r:id="rId2"/>
     <sheet name="4.3" sheetId="17" r:id="rId3"/>
-    <sheet name="total 4.1 to 4.6" sheetId="7" r:id="rId4"/>
+    <sheet name="4.4" sheetId="18" r:id="rId4"/>
+    <sheet name="total 4.1 to 4.6" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="222">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1788,6 +1789,117 @@
   </si>
   <si>
     <t>36</t>
+  </si>
+  <si>
+    <t>4.4.1.1 :</t>
+  </si>
+  <si>
+    <t>4.4.1.2 :</t>
+  </si>
+  <si>
+    <t>4.4.1.3 :</t>
+  </si>
+  <si>
+    <t>4.4.2.1 :</t>
+  </si>
+  <si>
+    <t>4.4.2.2 :</t>
+  </si>
+  <si>
+    <t>4.4.2.3 :</t>
+  </si>
+  <si>
+    <t>4.4.3.1 :</t>
+  </si>
+  <si>
+    <t>4.4.3.2 :</t>
+  </si>
+  <si>
+    <t>4.4.3.3 :</t>
+  </si>
+  <si>
+    <t>4.4.4.1 :</t>
+  </si>
+  <si>
+    <t>4.4.4.2 :</t>
+  </si>
+  <si>
+    <t>4.4.4.3 :</t>
+  </si>
+  <si>
+    <t>4.4.4.4 :</t>
+  </si>
+  <si>
+    <t>4.4.4.5 :</t>
+  </si>
+  <si>
+    <t>4.4.4.6 :</t>
+  </si>
+  <si>
+    <t>4.4.4.7 :</t>
+  </si>
+  <si>
+    <t>4.4.4.8 :</t>
+  </si>
+  <si>
+    <t>4.4.5.1 :</t>
+  </si>
+  <si>
+    <t>4.4.5.2 :</t>
+  </si>
+  <si>
+    <t>4.4.6.1 :</t>
+  </si>
+  <si>
+    <t>4.4.6.2 :</t>
+  </si>
+  <si>
+    <t>4.4.7.1 :</t>
+  </si>
+  <si>
+    <t>4.4.7.2 :</t>
+  </si>
+  <si>
+    <t>4.4.8.1 :</t>
+  </si>
+  <si>
+    <t>4.4.9.1 :</t>
+  </si>
+  <si>
+    <t>4.4.10.1 :</t>
+  </si>
+  <si>
+    <t>4.4.10.2 :</t>
+  </si>
+  <si>
+    <t>4.4.10.3 :</t>
+  </si>
+  <si>
+    <t>4.4.11.1 :</t>
+  </si>
+  <si>
+    <t>4.4.11.2 :</t>
+  </si>
+  <si>
+    <t>4.4.11.3 :</t>
+  </si>
+  <si>
+    <t>4.4.11.4 :</t>
+  </si>
+  <si>
+    <t>4.4.12.1 :</t>
+  </si>
+  <si>
+    <t>4.4.12.2 :</t>
+  </si>
+  <si>
+    <t>4.4.12.3 :</t>
+  </si>
+  <si>
+    <t>4.4.12.4 :</t>
+  </si>
+  <si>
+    <t>4.4.12.5 :</t>
   </si>
 </sst>
 </file>
@@ -6436,9 +6548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DC1F4F-BBB6-40F8-A352-CB08F5EFE478}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L38"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39:K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8003,6 +8115,1626 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A106FB53-1904-4C9F-908E-EFE882336702}">
+  <dimension ref="A1:L49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="3">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>43</v>
+      </c>
+      <c r="K2" s="3">
+        <v>50</v>
+      </c>
+      <c r="L2" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>38</v>
+      </c>
+      <c r="K3" s="3">
+        <v>50</v>
+      </c>
+      <c r="L3" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="3">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>28</v>
+      </c>
+      <c r="K4" s="3">
+        <v>43</v>
+      </c>
+      <c r="L4" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="3">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>39</v>
+      </c>
+      <c r="K5" s="3">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="3">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>39</v>
+      </c>
+      <c r="K6" s="3">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="3">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>26</v>
+      </c>
+      <c r="K7" s="3">
+        <v>40</v>
+      </c>
+      <c r="L7" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="3">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>30</v>
+      </c>
+      <c r="K8" s="3">
+        <v>50</v>
+      </c>
+      <c r="L8" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="3">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>35</v>
+      </c>
+      <c r="K9" s="3">
+        <v>50</v>
+      </c>
+      <c r="L9" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="3">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>65</v>
+      </c>
+      <c r="K10" s="3">
+        <v>78</v>
+      </c>
+      <c r="L10" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>39</v>
+      </c>
+      <c r="K11" s="3">
+        <v>50</v>
+      </c>
+      <c r="L11" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3">
+        <v>4</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>37</v>
+      </c>
+      <c r="K12" s="3">
+        <v>50</v>
+      </c>
+      <c r="L12" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3">
+        <v>4</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>38</v>
+      </c>
+      <c r="K13" s="3">
+        <v>50</v>
+      </c>
+      <c r="L13" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>7</v>
+      </c>
+      <c r="G14" s="3">
+        <v>4</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>38</v>
+      </c>
+      <c r="K14" s="3">
+        <v>50</v>
+      </c>
+      <c r="L14" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>34</v>
+      </c>
+      <c r="K15" s="3">
+        <v>50</v>
+      </c>
+      <c r="L15" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B16" s="3">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>6</v>
+      </c>
+      <c r="G16" s="3">
+        <v>6</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>34</v>
+      </c>
+      <c r="K16" s="3">
+        <v>50</v>
+      </c>
+      <c r="L16" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>7</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>42</v>
+      </c>
+      <c r="K17" s="3">
+        <v>50</v>
+      </c>
+      <c r="L17" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>37</v>
+      </c>
+      <c r="K18" s="3">
+        <v>55</v>
+      </c>
+      <c r="L18" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" s="3">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>39</v>
+      </c>
+      <c r="K19" s="3">
+        <v>50</v>
+      </c>
+      <c r="L19" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="3">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>43</v>
+      </c>
+      <c r="K20" s="3">
+        <v>48</v>
+      </c>
+      <c r="L20" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="3">
+        <v>14</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
+        <v>36</v>
+      </c>
+      <c r="K21" s="3">
+        <v>50</v>
+      </c>
+      <c r="L21" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="3">
+        <v>12</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>66</v>
+      </c>
+      <c r="K22" s="3">
+        <v>79</v>
+      </c>
+      <c r="L22" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="3">
+        <v>12</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>38</v>
+      </c>
+      <c r="K23" s="3">
+        <v>50</v>
+      </c>
+      <c r="L23" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="3">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>28</v>
+      </c>
+      <c r="K24" s="3">
+        <v>32</v>
+      </c>
+      <c r="L24" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="3">
+        <v>16</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>32</v>
+      </c>
+      <c r="K25" s="3">
+        <v>49</v>
+      </c>
+      <c r="L25" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="3">
+        <v>35</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <v>35</v>
+      </c>
+      <c r="K26" s="3">
+        <v>71</v>
+      </c>
+      <c r="L26" s="3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B27" s="3">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <v>44</v>
+      </c>
+      <c r="K27" s="3">
+        <v>50</v>
+      </c>
+      <c r="L27" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>45</v>
+      </c>
+      <c r="K28" s="3">
+        <v>50</v>
+      </c>
+      <c r="L28" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="3">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>26</v>
+      </c>
+      <c r="K29" s="3">
+        <v>33</v>
+      </c>
+      <c r="L29" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>41</v>
+      </c>
+      <c r="K30" s="3">
+        <v>50</v>
+      </c>
+      <c r="L30" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B31" s="3">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>3</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>44</v>
+      </c>
+      <c r="K31" s="3">
+        <v>50</v>
+      </c>
+      <c r="L31" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32" s="3">
+        <v>5</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>45</v>
+      </c>
+      <c r="K32" s="3">
+        <v>50</v>
+      </c>
+      <c r="L32" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="3">
+        <v>11</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
+        <v>33</v>
+      </c>
+      <c r="K33" s="3">
+        <v>45</v>
+      </c>
+      <c r="L33" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" s="3">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <v>36</v>
+      </c>
+      <c r="K34" s="3">
+        <v>50</v>
+      </c>
+      <c r="L34" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B35" s="3">
+        <v>8</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>6</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <v>38</v>
+      </c>
+      <c r="K35" s="3">
+        <v>50</v>
+      </c>
+      <c r="L35" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B36" s="3">
+        <v>14</v>
+      </c>
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>6</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
+      <c r="J36" s="3">
+        <v>30</v>
+      </c>
+      <c r="K36" s="3">
+        <v>50</v>
+      </c>
+      <c r="L36" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" s="3">
+        <v>9</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>36</v>
+      </c>
+      <c r="K37" s="3">
+        <v>50</v>
+      </c>
+      <c r="L37" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" s="3">
+        <v>11</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>7</v>
+      </c>
+      <c r="G38" s="3">
+        <v>4</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>48</v>
+      </c>
+      <c r="K38" s="3">
+        <v>64</v>
+      </c>
+      <c r="L38" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="31">
+        <v>37</v>
+      </c>
+      <c r="B39" s="35">
+        <f>SUM(B2:B38)</f>
+        <v>356</v>
+      </c>
+      <c r="C39" s="35">
+        <f t="shared" ref="C39:L39" si="0">SUM(C2:C38)</f>
+        <v>17</v>
+      </c>
+      <c r="D39" s="35">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E39" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="35">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="G39" s="35">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="H39" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I39" s="35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J39" s="35">
+        <f t="shared" si="0"/>
+        <v>1425</v>
+      </c>
+      <c r="K39" s="35">
+        <f t="shared" si="0"/>
+        <v>1887</v>
+      </c>
+      <c r="L39" s="35">
+        <f t="shared" si="0"/>
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40">
+        <f>G39</f>
+        <v>45</v>
+      </c>
+      <c r="J40">
+        <f>B39-C39</f>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41">
+        <f>B39</f>
+        <v>356</v>
+      </c>
+      <c r="J41">
+        <f>D39-E39</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42">
+        <v>18</v>
+      </c>
+      <c r="J42">
+        <f>F48</f>
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44">
+        <f>SUM(J40:J43)</f>
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f>SUM(F40:F44)</f>
+        <v>424</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46">
+        <f>K39-F45</f>
+        <v>1463</v>
+      </c>
+      <c r="J46">
+        <f>J44-L39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f>F46+F45</f>
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f>F48-K39</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:K31"/>
   <sheetViews>
@@ -8500,7 +10232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="99" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:11" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
@@ -8521,7 +10253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="99" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:11" ht="64.5" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
         <v>30</v>
       </c>

</xml_diff>